<commit_message>
final push before preprint; implemented all figures in one ipynb file, edited/verified Chris' original peak picks for fig4
</commit_message>
<xml_diff>
--- a/results/soae/Human Peak Picks (Fig.4)/Mags vs C_xi_M Picked Peaks.xlsx
+++ b/results/soae/Human Peak Picks (Fig.4)/Mags vs C_xi_M Picked Peaks.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -675,7 +675,7 @@
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="n">
-        <v>4.1630859375</v>
+        <v>4.40712890625</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -691,7 +691,7 @@
     <row r="14">
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="n">
-        <v>4.40712890625</v>
+        <v>5.55556640625</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -707,7 +707,7 @@
     <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="n">
-        <v>5.55556640625</v>
+        <v>6.47431640625</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
@@ -723,7 +723,7 @@
     <row r="16">
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="n">
-        <v>6.47431640625</v>
+        <v>7.6658203125</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
@@ -739,7 +739,7 @@
     <row r="17">
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="n">
-        <v>7.6658203125</v>
+        <v>11.7140625</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
@@ -754,10 +754,10 @@
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="n">
-        <v>11.7140625</v>
-      </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>0.67470703125</v>
+      </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -772,7 +772,7 @@
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
-        <v>0.67470703125</v>
+        <v>0.90439453125</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
@@ -788,7 +788,7 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="n">
-        <v>0.90439453125</v>
+        <v>1.435546875</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
@@ -804,7 +804,7 @@
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
-        <v>1.435546875</v>
+        <v>1.5216796875</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
@@ -820,7 +820,7 @@
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
-        <v>1.5216796875</v>
+        <v>1.665234375</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
@@ -836,7 +836,7 @@
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
-        <v>1.665234375</v>
+        <v>2.0384765625</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
@@ -852,7 +852,7 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="n">
-        <v>2.0384765625</v>
+        <v>2.28251953125</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -868,7 +868,7 @@
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
-        <v>2.28251953125</v>
+        <v>2.698828125</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
@@ -884,7 +884,7 @@
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="n">
-        <v>2.698828125</v>
+        <v>6.04365234375</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -899,10 +899,10 @@
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
-      <c r="C27" t="n">
-        <v>6.04365234375</v>
-      </c>
-      <c r="D27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="n">
+        <v>1.22021484375</v>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
@@ -917,7 +917,7 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>1.22021484375</v>
+        <v>1.49296875</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -933,7 +933,7 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>1.49296875</v>
+        <v>1.88056640625</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
@@ -949,7 +949,7 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>1.88056640625</v>
+        <v>3.78984375</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -964,10 +964,10 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="n">
-        <v>3.78984375</v>
-      </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="n">
+        <v>0.57421875</v>
+      </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
@@ -982,7 +982,7 @@
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>0.35888671875</v>
+        <v>1.1771484375</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -998,7 +998,7 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>0.57421875</v>
+        <v>1.36376953125</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
@@ -1014,7 +1014,7 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>1.1771484375</v>
+        <v>1.780078125</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
@@ -1030,7 +1030,7 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>1.36376953125</v>
+        <v>2.0384765625</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
@@ -1046,7 +1046,7 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>1.780078125</v>
+        <v>2.39736328125</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
@@ -1062,7 +1062,7 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>2.0384765625</v>
+        <v>2.54091796875</v>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
@@ -1078,7 +1078,7 @@
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>2.3830078125</v>
+        <v>2.698828125</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
@@ -1094,7 +1094,7 @@
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="n">
-        <v>2.54091796875</v>
+        <v>2.928515625</v>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -1110,7 +1110,7 @@
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
-        <v>2.698828125</v>
+        <v>3.71806640625</v>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
@@ -1126,7 +1126,7 @@
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
-        <v>2.928515625</v>
+        <v>3.91904296875</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
@@ -1141,10 +1141,10 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
-      <c r="E42" t="n">
-        <v>3.71806640625</v>
-      </c>
-      <c r="F42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>1.5791015625</v>
+      </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
@@ -1157,10 +1157,10 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
-      <c r="E43" t="n">
-        <v>3.91904296875</v>
-      </c>
-      <c r="F43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="n">
+        <v>3.6462890625</v>
+      </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
@@ -1175,7 +1175,7 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="n">
-        <v>1.5791015625</v>
+        <v>3.86162109375</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr"/>
@@ -1191,7 +1191,7 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
-        <v>3.6462890625</v>
+        <v>4.17744140625</v>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
@@ -1207,7 +1207,7 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="n">
-        <v>3.86162109375</v>
+        <v>4.69423828125</v>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
@@ -1223,7 +1223,7 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
-        <v>4.17744140625</v>
+        <v>7.04853515625</v>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
@@ -1239,7 +1239,7 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
-        <v>4.69423828125</v>
+        <v>7.33564453125</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
@@ -1255,7 +1255,7 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
-        <v>7.04853515625</v>
+        <v>9.07265625</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
@@ -1270,10 +1270,10 @@
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" t="n">
-        <v>7.33564453125</v>
-      </c>
-      <c r="G50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="n">
+        <v>1.4068359375</v>
+      </c>
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr"/>
@@ -1286,10 +1286,10 @@
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" t="n">
-        <v>9.07265625</v>
-      </c>
-      <c r="G51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="n">
+        <v>1.72265625</v>
+      </c>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
@@ -1304,7 +1304,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
-        <v>1.4068359375</v>
+        <v>1.88056640625</v>
       </c>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
@@ -1320,7 +1320,7 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="n">
-        <v>1.72265625</v>
+        <v>2.009765625</v>
       </c>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
@@ -1336,7 +1336,7 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
-        <v>1.88056640625</v>
+        <v>2.13896484375</v>
       </c>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
@@ -1352,7 +1352,7 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
-        <v>2.009765625</v>
+        <v>2.296875</v>
       </c>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
@@ -1368,7 +1368,7 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="n">
-        <v>2.13896484375</v>
+        <v>2.45478515625</v>
       </c>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr"/>
@@ -1384,7 +1384,7 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="n">
-        <v>2.296875</v>
+        <v>2.6126953125</v>
       </c>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
@@ -1400,7 +1400,7 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="n">
-        <v>2.45478515625</v>
+        <v>2.75625</v>
       </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
@@ -1416,7 +1416,7 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="n">
-        <v>2.6126953125</v>
+        <v>3.0720703125</v>
       </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
@@ -1432,7 +1432,7 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="n">
-        <v>2.75625</v>
+        <v>3.273046875</v>
       </c>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr"/>
@@ -1448,7 +1448,7 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="n">
-        <v>3.0720703125</v>
+        <v>4.134375</v>
       </c>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
@@ -1463,10 +1463,10 @@
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
-      <c r="G62" t="n">
-        <v>3.273046875</v>
-      </c>
-      <c r="H62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="n">
+        <v>1.70830078125</v>
+      </c>
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
@@ -1479,10 +1479,10 @@
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
-      <c r="G63" t="n">
-        <v>4.134375</v>
-      </c>
-      <c r="H63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="n">
+        <v>1.85185546875</v>
+      </c>
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
@@ -1497,7 +1497,7 @@
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
-        <v>1.70830078125</v>
+        <v>2.239453125</v>
       </c>
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr"/>
@@ -1513,7 +1513,7 @@
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
-        <v>1.85185546875</v>
+        <v>2.42607421875</v>
       </c>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
@@ -1529,7 +1529,7 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>2.239453125</v>
+        <v>2.45478515625</v>
       </c>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
@@ -1545,7 +1545,7 @@
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
-        <v>2.42607421875</v>
+        <v>2.64140625</v>
       </c>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
@@ -1561,7 +1561,7 @@
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>2.45478515625</v>
+        <v>2.9859375</v>
       </c>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
@@ -1577,7 +1577,7 @@
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>2.64140625</v>
+        <v>3.54580078125</v>
       </c>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
@@ -1593,7 +1593,7 @@
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
-        <v>2.9859375</v>
+        <v>4.34970703125</v>
       </c>
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
@@ -1609,7 +1609,7 @@
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>3.54580078125</v>
+        <v>6.5748046875</v>
       </c>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
@@ -1624,10 +1624,10 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
-      <c r="H72" t="n">
-        <v>4.34970703125</v>
-      </c>
-      <c r="I72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="n">
+        <v>1.550390625</v>
+      </c>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
@@ -1640,10 +1640,10 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
-      <c r="H73" t="n">
-        <v>6.5748046875</v>
-      </c>
-      <c r="I73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="n">
+        <v>1.72265625</v>
+      </c>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
@@ -1658,7 +1658,7 @@
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="n">
-        <v>0.30146484375</v>
+        <v>2.02412109375</v>
       </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
@@ -1674,7 +1674,7 @@
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="n">
-        <v>1.550390625</v>
+        <v>2.239453125</v>
       </c>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
@@ -1690,7 +1690,7 @@
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="n">
-        <v>1.72265625</v>
+        <v>2.75625</v>
       </c>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
@@ -1706,7 +1706,7 @@
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="n">
-        <v>2.02412109375</v>
+        <v>3.043359375</v>
       </c>
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
@@ -1722,7 +1722,7 @@
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="n">
-        <v>2.239453125</v>
+        <v>3.17255859375</v>
       </c>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
@@ -1738,7 +1738,7 @@
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="n">
-        <v>2.75625</v>
+        <v>4.00517578125</v>
       </c>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
@@ -1753,10 +1753,10 @@
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
-      <c r="I80" t="n">
-        <v>3.043359375</v>
-      </c>
-      <c r="J80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="n">
+        <v>1.2345703125</v>
+      </c>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
     </row>
@@ -1769,10 +1769,10 @@
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
-      <c r="I81" t="n">
-        <v>3.17255859375</v>
-      </c>
-      <c r="J81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="n">
+        <v>1.435546875</v>
+      </c>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
     </row>
@@ -1785,10 +1785,10 @@
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
-      <c r="I82" t="n">
-        <v>4.00517578125</v>
-      </c>
-      <c r="J82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="n">
+        <v>1.6939453125</v>
+      </c>
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr"/>
     </row>
@@ -1803,7 +1803,7 @@
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="n">
-        <v>1.2345703125</v>
+        <v>1.96669921875</v>
       </c>
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr"/>
@@ -1819,7 +1819,7 @@
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="n">
-        <v>1.44990234375</v>
+        <v>3.56015625</v>
       </c>
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr"/>
@@ -1835,7 +1835,7 @@
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="inlineStr"/>
       <c r="J85" t="n">
-        <v>1.6939453125</v>
+        <v>4.06259765625</v>
       </c>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
@@ -1851,7 +1851,7 @@
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="n">
-        <v>1.96669921875</v>
+        <v>7.27822265625</v>
       </c>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr"/>
@@ -1866,10 +1866,10 @@
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr"/>
-      <c r="J87" t="n">
-        <v>3.56015625</v>
-      </c>
-      <c r="K87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="n">
+        <v>0.73212890625</v>
+      </c>
       <c r="L87" t="inlineStr"/>
     </row>
     <row r="88">
@@ -1882,10 +1882,10 @@
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr"/>
-      <c r="J88" t="n">
-        <v>4.06259765625</v>
-      </c>
-      <c r="K88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="n">
+        <v>0.99052734375</v>
+      </c>
       <c r="L88" t="inlineStr"/>
     </row>
     <row r="89">
@@ -1898,10 +1898,10 @@
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
       <c r="I89" t="inlineStr"/>
-      <c r="J89" t="n">
-        <v>7.27822265625</v>
-      </c>
-      <c r="K89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="n">
+        <v>1.6365234375</v>
+      </c>
       <c r="L89" t="inlineStr"/>
     </row>
     <row r="90">
@@ -1916,7 +1916,7 @@
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="n">
-        <v>0.73212890625</v>
+        <v>2.22509765625</v>
       </c>
       <c r="L90" t="inlineStr"/>
     </row>
@@ -1932,7 +1932,7 @@
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="n">
-        <v>0.99052734375</v>
+        <v>3.11513671875</v>
       </c>
       <c r="L91" t="inlineStr"/>
     </row>
@@ -1947,10 +1947,10 @@
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr"/>
-      <c r="K92" t="n">
+      <c r="K92" t="inlineStr"/>
+      <c r="L92" t="n">
         <v>1.2919921875</v>
       </c>
-      <c r="L92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr"/>
@@ -1963,10 +1963,10 @@
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr"/>
-      <c r="K93" t="n">
-        <v>1.6365234375</v>
-      </c>
-      <c r="L93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="n">
+        <v>1.72265625</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr"/>
@@ -1979,10 +1979,10 @@
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr"/>
       <c r="J94" t="inlineStr"/>
-      <c r="K94" t="n">
-        <v>2.2107421875</v>
-      </c>
-      <c r="L94" t="inlineStr"/>
+      <c r="K94" t="inlineStr"/>
+      <c r="L94" t="n">
+        <v>1.8375</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr"/>
@@ -1995,10 +1995,10 @@
       <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr"/>
-      <c r="K95" t="n">
-        <v>3.11513671875</v>
-      </c>
-      <c r="L95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="n">
+        <v>2.33994140625</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr"/>
@@ -2013,7 +2013,7 @@
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="n">
-        <v>1.2919921875</v>
+        <v>2.813671875</v>
       </c>
     </row>
     <row r="97">
@@ -2029,7 +2029,7 @@
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="n">
-        <v>1.72265625</v>
+        <v>3.40224609375</v>
       </c>
     </row>
     <row r="98">
@@ -2045,7 +2045,7 @@
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="n">
-        <v>1.8375</v>
+        <v>4.0482421875</v>
       </c>
     </row>
     <row r="99">
@@ -2061,7 +2061,7 @@
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="n">
-        <v>2.33994140625</v>
+        <v>5.12490234375</v>
       </c>
     </row>
     <row r="100">
@@ -2077,7 +2077,7 @@
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="n">
-        <v>2.813671875</v>
+        <v>5.84267578125</v>
       </c>
     </row>
     <row r="101">
@@ -2093,7 +2093,7 @@
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="n">
-        <v>3.40224609375</v>
+        <v>7.93857421875</v>
       </c>
     </row>
     <row r="102">
@@ -2109,7 +2109,7 @@
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="n">
-        <v>4.0482421875</v>
+        <v>8.311816406249999</v>
       </c>
     </row>
     <row r="103">
@@ -2125,70 +2125,6 @@
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="n">
-        <v>5.12490234375</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr"/>
-      <c r="B104" t="inlineStr"/>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
-      <c r="I104" t="inlineStr"/>
-      <c r="J104" t="inlineStr"/>
-      <c r="K104" t="inlineStr"/>
-      <c r="L104" t="n">
-        <v>5.84267578125</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr"/>
-      <c r="B105" t="inlineStr"/>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr"/>
-      <c r="H105" t="inlineStr"/>
-      <c r="I105" t="inlineStr"/>
-      <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr"/>
-      <c r="L105" t="n">
-        <v>7.93857421875</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr"/>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr"/>
-      <c r="H106" t="inlineStr"/>
-      <c r="I106" t="inlineStr"/>
-      <c r="J106" t="inlineStr"/>
-      <c r="K106" t="inlineStr"/>
-      <c r="L106" t="n">
-        <v>8.311816406249999</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr"/>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr"/>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
-      <c r="I107" t="inlineStr"/>
-      <c r="J107" t="inlineStr"/>
-      <c r="K107" t="inlineStr"/>
-      <c r="L107" t="n">
         <v>8.68505859375</v>
       </c>
     </row>
@@ -2203,7 +2139,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L219"/>
+  <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2291,7 +2227,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.70341796875</v>
+        <v>0.861328125</v>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
@@ -2307,7 +2243,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.861328125</v>
+        <v>0.93310546875</v>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
@@ -2323,7 +2259,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.93310546875</v>
+        <v>1.1197265625</v>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
@@ -2339,7 +2275,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.1197265625</v>
+        <v>1.19150390625</v>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
@@ -2355,7 +2291,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.19150390625</v>
+        <v>1.26328125</v>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
@@ -2371,7 +2307,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.26328125</v>
+        <v>1.3494140625</v>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
@@ -2387,7 +2323,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.3494140625</v>
+        <v>1.53603515625</v>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
@@ -2403,7 +2339,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.53603515625</v>
+        <v>1.62216796875</v>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
@@ -2419,7 +2355,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.62216796875</v>
+        <v>2.25380859375</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
@@ -2435,7 +2371,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2.25380859375</v>
+        <v>2.82802734375</v>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
@@ -2451,7 +2387,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2.698828125</v>
+        <v>3.08642578125</v>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
@@ -2467,7 +2403,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2.82802734375</v>
+        <v>3.4453125</v>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
@@ -2483,7 +2419,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3.08642578125</v>
+        <v>4.37841796875</v>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
@@ -2499,7 +2435,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.4453125</v>
+        <v>4.52197265625</v>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
@@ -2515,7 +2451,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.86162109375</v>
+        <v>4.72294921875</v>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
@@ -2531,7 +2467,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>4.37841796875</v>
+        <v>6.0580078125</v>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
@@ -2547,7 +2483,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>4.52197265625</v>
+        <v>6.31640625</v>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
@@ -2562,10 +2498,10 @@
       <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>4.72294921875</v>
-      </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="n">
+        <v>2.13896484375</v>
+      </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
@@ -2578,10 +2514,10 @@
       <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>6.0580078125</v>
-      </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="n">
+        <v>3.25869140625</v>
+      </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
@@ -2594,10 +2530,10 @@
       <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>6.31640625</v>
-      </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="n">
+        <v>3.732421875</v>
+      </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
@@ -2612,7 +2548,7 @@
     <row r="23">
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="n">
-        <v>1.67958984375</v>
+        <v>4.1630859375</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
@@ -2628,7 +2564,7 @@
     <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="n">
-        <v>2.13896484375</v>
+        <v>4.40712890625</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
@@ -2644,7 +2580,7 @@
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="n">
-        <v>2.469140625</v>
+        <v>5.55556640625</v>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
@@ -2660,7 +2596,7 @@
     <row r="26">
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="n">
-        <v>3.25869140625</v>
+        <v>6.47431640625</v>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
@@ -2676,7 +2612,7 @@
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="n">
-        <v>3.732421875</v>
+        <v>7.6658203125</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
@@ -2692,7 +2628,7 @@
     <row r="28">
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="n">
-        <v>4.1630859375</v>
+        <v>11.7140625</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
@@ -2707,10 +2643,10 @@
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
-      <c r="B29" t="n">
-        <v>4.40712890625</v>
-      </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="n">
+        <v>0.3732421875</v>
+      </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
@@ -2723,10 +2659,10 @@
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
-      <c r="B30" t="n">
-        <v>5.55556640625</v>
-      </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="n">
+        <v>0.64599609375</v>
+      </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -2739,10 +2675,10 @@
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
-      <c r="B31" t="n">
-        <v>6.47431640625</v>
-      </c>
-      <c r="C31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="n">
+        <v>0.84697265625</v>
+      </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
@@ -2755,10 +2691,10 @@
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
-      <c r="B32" t="n">
-        <v>7.6658203125</v>
-      </c>
-      <c r="C32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="n">
+        <v>0.90439453125</v>
+      </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
@@ -2771,10 +2707,10 @@
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
-      <c r="B33" t="n">
-        <v>7.8380859375</v>
-      </c>
-      <c r="C33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="n">
+        <v>0.976171875</v>
+      </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
@@ -2787,10 +2723,10 @@
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
-      <c r="B34" t="n">
-        <v>8.36923828125</v>
-      </c>
-      <c r="C34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="n">
+        <v>1.091015625</v>
+      </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
@@ -2803,10 +2739,10 @@
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
-      <c r="B35" t="n">
-        <v>8.4984375</v>
-      </c>
-      <c r="C35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="n">
+        <v>1.27763671875</v>
+      </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
@@ -2819,10 +2755,10 @@
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
-      <c r="B36" t="n">
-        <v>9.847851562500001</v>
-      </c>
-      <c r="C36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="n">
+        <v>1.33505859375</v>
+      </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
@@ -2835,10 +2771,10 @@
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
-      <c r="B37" t="n">
-        <v>11.7140625</v>
-      </c>
-      <c r="C37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="n">
+        <v>1.435546875</v>
+      </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
@@ -2853,7 +2789,7 @@
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="n">
-        <v>0.3732421875</v>
+        <v>1.5216796875</v>
       </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
@@ -2869,7 +2805,7 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="n">
-        <v>0.64599609375</v>
+        <v>1.59345703125</v>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
@@ -2885,7 +2821,7 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="n">
-        <v>0.84697265625</v>
+        <v>1.67958984375</v>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
@@ -2901,7 +2837,7 @@
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="n">
-        <v>0.90439453125</v>
+        <v>1.8087890625</v>
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
@@ -2917,7 +2853,7 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="n">
-        <v>0.976171875</v>
+        <v>1.9236328125</v>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
@@ -2933,7 +2869,7 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="n">
-        <v>1.091015625</v>
+        <v>2.0384765625</v>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
@@ -2949,7 +2885,7 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="n">
-        <v>1.27763671875</v>
+        <v>2.1533203125</v>
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
@@ -2965,7 +2901,7 @@
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="n">
-        <v>1.33505859375</v>
+        <v>2.28251953125</v>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
@@ -2981,7 +2917,7 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="n">
-        <v>1.435546875</v>
+        <v>2.698828125</v>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
@@ -2997,7 +2933,7 @@
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="n">
-        <v>1.5216796875</v>
+        <v>2.8423828125</v>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
@@ -3013,7 +2949,7 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="n">
-        <v>1.59345703125</v>
+        <v>3.63193359375</v>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
@@ -3029,7 +2965,7 @@
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="n">
-        <v>1.67958984375</v>
+        <v>6.04365234375</v>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
@@ -3045,7 +2981,7 @@
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="n">
-        <v>1.8087890625</v>
+        <v>7.292578125</v>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
@@ -3060,10 +2996,10 @@
     <row r="51">
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
-      <c r="C51" t="n">
-        <v>1.9236328125</v>
-      </c>
-      <c r="D51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>0.70341796875</v>
+      </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
@@ -3076,10 +3012,10 @@
     <row r="52">
       <c r="A52" t="inlineStr"/>
       <c r="B52" t="inlineStr"/>
-      <c r="C52" t="n">
-        <v>2.0384765625</v>
-      </c>
-      <c r="D52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>0.87568359375</v>
+      </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
@@ -3092,10 +3028,10 @@
     <row r="53">
       <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr"/>
-      <c r="C53" t="n">
-        <v>2.1533203125</v>
-      </c>
-      <c r="D53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>1.10537109375</v>
+      </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
@@ -3108,10 +3044,10 @@
     <row r="54">
       <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr"/>
-      <c r="C54" t="n">
-        <v>2.28251953125</v>
-      </c>
-      <c r="D54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>1.22021484375</v>
+      </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
@@ -3124,10 +3060,10 @@
     <row r="55">
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr"/>
-      <c r="C55" t="n">
-        <v>2.698828125</v>
-      </c>
-      <c r="D55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>1.3494140625</v>
+      </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
@@ -3140,10 +3076,10 @@
     <row r="56">
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr"/>
-      <c r="C56" t="n">
-        <v>2.8423828125</v>
-      </c>
-      <c r="D56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>1.49296875</v>
+      </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
@@ -3156,10 +3092,10 @@
     <row r="57">
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr"/>
-      <c r="C57" t="n">
-        <v>3.63193359375</v>
-      </c>
-      <c r="D57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>1.88056640625</v>
+      </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
@@ -3172,10 +3108,10 @@
     <row r="58">
       <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr"/>
-      <c r="C58" t="n">
-        <v>6.04365234375</v>
-      </c>
-      <c r="D58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>3.043359375</v>
+      </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
@@ -3188,10 +3124,10 @@
     <row r="59">
       <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr"/>
-      <c r="C59" t="n">
-        <v>7.292578125</v>
-      </c>
-      <c r="D59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>3.158203125</v>
+      </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
@@ -3206,7 +3142,7 @@
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="n">
-        <v>0.6603515625</v>
+        <v>3.3017578125</v>
       </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
@@ -3222,7 +3158,7 @@
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="n">
-        <v>0.70341796875</v>
+        <v>3.78984375</v>
       </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
@@ -3237,10 +3173,10 @@
       <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="n">
-        <v>0.87568359375</v>
-      </c>
-      <c r="E62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="n">
+        <v>0.3732421875</v>
+      </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
@@ -3253,10 +3189,10 @@
       <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="n">
-        <v>1.10537109375</v>
-      </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>0.58857421875</v>
+      </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
@@ -3269,10 +3205,10 @@
       <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="n">
-        <v>1.16279296875</v>
-      </c>
-      <c r="E64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>0.6890625</v>
+      </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
@@ -3285,10 +3221,10 @@
       <c r="A65" t="inlineStr"/>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="n">
-        <v>1.22021484375</v>
-      </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>0.78955078125</v>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
@@ -3301,10 +3237,10 @@
       <c r="A66" t="inlineStr"/>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="n">
-        <v>1.3494140625</v>
-      </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>0.861328125</v>
+      </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
@@ -3317,10 +3253,10 @@
       <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="n">
-        <v>1.49296875</v>
-      </c>
-      <c r="E67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>1.1771484375</v>
+      </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
@@ -3333,10 +3269,10 @@
       <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="n">
-        <v>1.88056640625</v>
-      </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="n">
+        <v>1.26328125</v>
+      </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
@@ -3349,10 +3285,10 @@
       <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="n">
-        <v>3.043359375</v>
-      </c>
-      <c r="E69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>1.36376953125</v>
+      </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
@@ -3365,10 +3301,10 @@
       <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
-      <c r="D70" t="n">
-        <v>3.158203125</v>
-      </c>
-      <c r="E70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="n">
+        <v>1.79443359375</v>
+      </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
@@ -3381,10 +3317,10 @@
       <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="n">
-        <v>3.3017578125</v>
-      </c>
-      <c r="E71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>2.0384765625</v>
+      </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
@@ -3397,10 +3333,10 @@
       <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="n">
-        <v>3.78984375</v>
-      </c>
-      <c r="E72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>2.16767578125</v>
+      </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
@@ -3415,7 +3351,7 @@
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
-        <v>0.3732421875</v>
+        <v>2.296875</v>
       </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
@@ -3431,7 +3367,7 @@
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="n">
-        <v>0.58857421875</v>
+        <v>2.39736328125</v>
       </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
@@ -3447,7 +3383,7 @@
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="n">
-        <v>0.6890625</v>
+        <v>2.54091796875</v>
       </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
@@ -3463,7 +3399,7 @@
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
-        <v>0.78955078125</v>
+        <v>2.698828125</v>
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
@@ -3479,7 +3415,7 @@
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="n">
-        <v>0.861328125</v>
+        <v>2.928515625</v>
       </c>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
@@ -3495,7 +3431,7 @@
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="n">
-        <v>1.0623046875</v>
+        <v>3.11513671875</v>
       </c>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
@@ -3511,7 +3447,7 @@
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
-        <v>1.1771484375</v>
+        <v>3.71806640625</v>
       </c>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr"/>
@@ -3527,7 +3463,7 @@
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="n">
-        <v>1.26328125</v>
+        <v>3.91904296875</v>
       </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
@@ -3542,10 +3478,10 @@
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
-      <c r="E81" t="n">
-        <v>1.36376953125</v>
-      </c>
-      <c r="F81" t="inlineStr"/>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="n">
+        <v>0.57421875</v>
+      </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr"/>
@@ -3558,10 +3494,10 @@
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
-      <c r="E82" t="n">
-        <v>1.79443359375</v>
-      </c>
-      <c r="F82" t="inlineStr"/>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="n">
+        <v>0.61728515625</v>
+      </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr"/>
@@ -3574,10 +3510,10 @@
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
-      <c r="E83" t="n">
-        <v>2.0384765625</v>
-      </c>
-      <c r="F83" t="inlineStr"/>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="n">
+        <v>0.73212890625</v>
+      </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
@@ -3590,10 +3526,10 @@
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
-      <c r="E84" t="n">
-        <v>2.16767578125</v>
-      </c>
-      <c r="F84" t="inlineStr"/>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="n">
+        <v>0.78955078125</v>
+      </c>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr"/>
@@ -3606,10 +3542,10 @@
       <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
-      <c r="E85" t="n">
-        <v>2.296875</v>
-      </c>
-      <c r="F85" t="inlineStr"/>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="n">
+        <v>0.91875</v>
+      </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="inlineStr"/>
@@ -3622,10 +3558,10 @@
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr"/>
-      <c r="E86" t="n">
-        <v>2.39736328125</v>
-      </c>
-      <c r="F86" t="inlineStr"/>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="n">
+        <v>0.99052734375</v>
+      </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="inlineStr"/>
@@ -3638,10 +3574,10 @@
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
-      <c r="E87" t="n">
-        <v>2.54091796875</v>
-      </c>
-      <c r="F87" t="inlineStr"/>
+      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="n">
+        <v>1.07666015625</v>
+      </c>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr"/>
@@ -3654,10 +3590,10 @@
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr"/>
-      <c r="E88" t="n">
-        <v>2.698828125</v>
-      </c>
-      <c r="F88" t="inlineStr"/>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="n">
+        <v>1.13408203125</v>
+      </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr"/>
@@ -3670,10 +3606,10 @@
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr"/>
-      <c r="E89" t="n">
-        <v>2.928515625</v>
-      </c>
-      <c r="F89" t="inlineStr"/>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="n">
+        <v>1.320703125</v>
+      </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
       <c r="I89" t="inlineStr"/>
@@ -3686,10 +3622,10 @@
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
-      <c r="E90" t="n">
-        <v>3.11513671875</v>
-      </c>
-      <c r="F90" t="inlineStr"/>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="n">
+        <v>1.50732421875</v>
+      </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr"/>
@@ -3702,10 +3638,10 @@
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr"/>
-      <c r="E91" t="n">
-        <v>3.71806640625</v>
-      </c>
-      <c r="F91" t="inlineStr"/>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="n">
+        <v>1.5791015625</v>
+      </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr"/>
@@ -3718,10 +3654,10 @@
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr"/>
-      <c r="E92" t="n">
-        <v>3.91904296875</v>
-      </c>
-      <c r="F92" t="inlineStr"/>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="n">
+        <v>1.665234375</v>
+      </c>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr"/>
@@ -3736,7 +3672,7 @@
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="n">
-        <v>0.57421875</v>
+        <v>3.6462890625</v>
       </c>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr"/>
@@ -3752,7 +3688,7 @@
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
       <c r="F94" t="n">
-        <v>0.61728515625</v>
+        <v>3.86162109375</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
@@ -3768,7 +3704,7 @@
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="n">
-        <v>0.73212890625</v>
+        <v>4.01953125</v>
       </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr"/>
@@ -3784,7 +3720,7 @@
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="n">
-        <v>0.78955078125</v>
+        <v>4.17744140625</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
@@ -3800,7 +3736,7 @@
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="n">
-        <v>0.91875</v>
+        <v>4.69423828125</v>
       </c>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr"/>
@@ -3816,7 +3752,7 @@
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="n">
-        <v>0.99052734375</v>
+        <v>5.6560546875</v>
       </c>
       <c r="G98" t="inlineStr"/>
       <c r="H98" t="inlineStr"/>
@@ -3832,7 +3768,7 @@
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
       <c r="F99" t="n">
-        <v>1.07666015625</v>
+        <v>6.76142578125</v>
       </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
@@ -3848,7 +3784,7 @@
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
       <c r="F100" t="n">
-        <v>1.13408203125</v>
+        <v>7.04853515625</v>
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
@@ -3864,7 +3800,7 @@
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="n">
-        <v>1.320703125</v>
+        <v>7.33564453125</v>
       </c>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
@@ -3880,7 +3816,7 @@
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="n">
-        <v>1.435546875</v>
+        <v>7.62275390625</v>
       </c>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr"/>
@@ -3896,7 +3832,7 @@
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="n">
-        <v>1.50732421875</v>
+        <v>9.07265625</v>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
@@ -3911,10 +3847,10 @@
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
-      <c r="F104" t="n">
-        <v>1.5791015625</v>
-      </c>
-      <c r="G104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="n">
+        <v>1.4068359375</v>
+      </c>
       <c r="H104" t="inlineStr"/>
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr"/>
@@ -3927,10 +3863,10 @@
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
-      <c r="F105" t="n">
-        <v>1.665234375</v>
-      </c>
-      <c r="G105" t="inlineStr"/>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="n">
+        <v>1.50732421875</v>
+      </c>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
@@ -3943,10 +3879,10 @@
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
-      <c r="F106" t="n">
-        <v>3.6462890625</v>
-      </c>
-      <c r="G106" t="inlineStr"/>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="n">
+        <v>1.62216796875</v>
+      </c>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr"/>
@@ -3959,10 +3895,10 @@
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
-      <c r="F107" t="n">
-        <v>3.86162109375</v>
-      </c>
-      <c r="G107" t="inlineStr"/>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="n">
+        <v>1.72265625</v>
+      </c>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr"/>
@@ -3975,10 +3911,10 @@
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
-      <c r="F108" t="n">
-        <v>4.01953125</v>
-      </c>
-      <c r="G108" t="inlineStr"/>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="n">
+        <v>1.88056640625</v>
+      </c>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr"/>
@@ -3991,10 +3927,10 @@
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
-      <c r="F109" t="n">
-        <v>4.17744140625</v>
-      </c>
-      <c r="G109" t="inlineStr"/>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="n">
+        <v>2.009765625</v>
+      </c>
       <c r="H109" t="inlineStr"/>
       <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr"/>
@@ -4007,10 +3943,10 @@
       <c r="C110" t="inlineStr"/>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
-      <c r="F110" t="n">
-        <v>4.49326171875</v>
-      </c>
-      <c r="G110" t="inlineStr"/>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="n">
+        <v>2.13896484375</v>
+      </c>
       <c r="H110" t="inlineStr"/>
       <c r="I110" t="inlineStr"/>
       <c r="J110" t="inlineStr"/>
@@ -4023,10 +3959,10 @@
       <c r="C111" t="inlineStr"/>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
-      <c r="F111" t="n">
-        <v>4.69423828125</v>
-      </c>
-      <c r="G111" t="inlineStr"/>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="n">
+        <v>2.296875</v>
+      </c>
       <c r="H111" t="inlineStr"/>
       <c r="I111" t="inlineStr"/>
       <c r="J111" t="inlineStr"/>
@@ -4039,10 +3975,10 @@
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
-      <c r="F112" t="n">
-        <v>5.6560546875</v>
-      </c>
-      <c r="G112" t="inlineStr"/>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="n">
+        <v>2.469140625</v>
+      </c>
       <c r="H112" t="inlineStr"/>
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
@@ -4055,10 +3991,10 @@
       <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
-      <c r="F113" t="n">
-        <v>6.76142578125</v>
-      </c>
-      <c r="G113" t="inlineStr"/>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="n">
+        <v>2.6126953125</v>
+      </c>
       <c r="H113" t="inlineStr"/>
       <c r="I113" t="inlineStr"/>
       <c r="J113" t="inlineStr"/>
@@ -4071,10 +4007,10 @@
       <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
-      <c r="F114" t="n">
-        <v>7.04853515625</v>
-      </c>
-      <c r="G114" t="inlineStr"/>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="n">
+        <v>2.75625</v>
+      </c>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
@@ -4087,10 +4023,10 @@
       <c r="C115" t="inlineStr"/>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
-      <c r="F115" t="n">
-        <v>7.33564453125</v>
-      </c>
-      <c r="G115" t="inlineStr"/>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="n">
+        <v>2.91416015625</v>
+      </c>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr"/>
@@ -4103,10 +4039,10 @@
       <c r="C116" t="inlineStr"/>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
-      <c r="F116" t="n">
-        <v>7.62275390625</v>
-      </c>
-      <c r="G116" t="inlineStr"/>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="n">
+        <v>3.0720703125</v>
+      </c>
       <c r="H116" t="inlineStr"/>
       <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr"/>
@@ -4119,10 +4055,10 @@
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
-      <c r="F117" t="n">
-        <v>9.07265625</v>
-      </c>
-      <c r="G117" t="inlineStr"/>
+      <c r="F117" t="inlineStr"/>
+      <c r="G117" t="n">
+        <v>3.273046875</v>
+      </c>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr"/>
@@ -4137,7 +4073,7 @@
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="n">
-        <v>1.4068359375</v>
+        <v>4.134375</v>
       </c>
       <c r="H118" t="inlineStr"/>
       <c r="I118" t="inlineStr"/>
@@ -4152,10 +4088,10 @@
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
-      <c r="G119" t="n">
-        <v>1.50732421875</v>
-      </c>
-      <c r="H119" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="n">
+        <v>0.6890625</v>
+      </c>
       <c r="I119" t="inlineStr"/>
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr"/>
@@ -4168,10 +4104,10 @@
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
-      <c r="G120" t="n">
-        <v>1.62216796875</v>
-      </c>
-      <c r="H120" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="n">
+        <v>1.26328125</v>
+      </c>
       <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr"/>
       <c r="K120" t="inlineStr"/>
@@ -4184,10 +4120,10 @@
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
       <c r="F121" t="inlineStr"/>
-      <c r="G121" t="n">
-        <v>1.72265625</v>
-      </c>
-      <c r="H121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="n">
+        <v>1.36376953125</v>
+      </c>
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr"/>
@@ -4200,10 +4136,10 @@
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr"/>
-      <c r="G122" t="n">
-        <v>1.88056640625</v>
-      </c>
-      <c r="H122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="n">
+        <v>1.56474609375</v>
+      </c>
       <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
@@ -4216,10 +4152,10 @@
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
-      <c r="G123" t="n">
-        <v>2.009765625</v>
-      </c>
-      <c r="H123" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="n">
+        <v>1.70830078125</v>
+      </c>
       <c r="I123" t="inlineStr"/>
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
@@ -4232,10 +4168,10 @@
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
-      <c r="G124" t="n">
-        <v>2.13896484375</v>
-      </c>
-      <c r="H124" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="n">
+        <v>1.85185546875</v>
+      </c>
       <c r="I124" t="inlineStr"/>
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr"/>
@@ -4248,10 +4184,10 @@
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
-      <c r="G125" t="n">
-        <v>2.296875</v>
-      </c>
-      <c r="H125" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="n">
+        <v>1.99541015625</v>
+      </c>
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr"/>
       <c r="K125" t="inlineStr"/>
@@ -4264,10 +4200,10 @@
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
-      <c r="G126" t="n">
-        <v>2.469140625</v>
-      </c>
-      <c r="H126" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="n">
+        <v>2.11025390625</v>
+      </c>
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr"/>
       <c r="K126" t="inlineStr"/>
@@ -4280,10 +4216,10 @@
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
-      <c r="G127" t="n">
-        <v>2.6126953125</v>
-      </c>
-      <c r="H127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="n">
+        <v>2.239453125</v>
+      </c>
       <c r="I127" t="inlineStr"/>
       <c r="J127" t="inlineStr"/>
       <c r="K127" t="inlineStr"/>
@@ -4296,10 +4232,10 @@
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
-      <c r="G128" t="n">
-        <v>2.75625</v>
-      </c>
-      <c r="H128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="n">
+        <v>2.41171875</v>
+      </c>
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr"/>
@@ -4312,10 +4248,10 @@
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
-      <c r="G129" t="n">
-        <v>2.91416015625</v>
-      </c>
-      <c r="H129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="n">
+        <v>2.45478515625</v>
+      </c>
       <c r="I129" t="inlineStr"/>
       <c r="J129" t="inlineStr"/>
       <c r="K129" t="inlineStr"/>
@@ -4328,10 +4264,10 @@
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
-      <c r="G130" t="n">
-        <v>3.0720703125</v>
-      </c>
-      <c r="H130" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="n">
+        <v>2.64140625</v>
+      </c>
       <c r="I130" t="inlineStr"/>
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="inlineStr"/>
@@ -4344,10 +4280,10 @@
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
-      <c r="G131" t="n">
-        <v>3.273046875</v>
-      </c>
-      <c r="H131" t="inlineStr"/>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="n">
+        <v>2.9859375</v>
+      </c>
       <c r="I131" t="inlineStr"/>
       <c r="J131" t="inlineStr"/>
       <c r="K131" t="inlineStr"/>
@@ -4360,10 +4296,10 @@
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
-      <c r="G132" t="n">
-        <v>4.134375</v>
-      </c>
-      <c r="H132" t="inlineStr"/>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="n">
+        <v>3.54580078125</v>
+      </c>
       <c r="I132" t="inlineStr"/>
       <c r="J132" t="inlineStr"/>
       <c r="K132" t="inlineStr"/>
@@ -4378,7 +4314,7 @@
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="n">
-        <v>0.6890625</v>
+        <v>4.34970703125</v>
       </c>
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr"/>
@@ -4394,7 +4330,7 @@
       <c r="F134" t="inlineStr"/>
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="n">
-        <v>1.26328125</v>
+        <v>6.5748046875</v>
       </c>
       <c r="I134" t="inlineStr"/>
       <c r="J134" t="inlineStr"/>
@@ -4409,10 +4345,10 @@
       <c r="E135" t="inlineStr"/>
       <c r="F135" t="inlineStr"/>
       <c r="G135" t="inlineStr"/>
-      <c r="H135" t="n">
-        <v>1.36376953125</v>
-      </c>
-      <c r="I135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="n">
+        <v>0.30146484375</v>
+      </c>
       <c r="J135" t="inlineStr"/>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr"/>
@@ -4425,10 +4361,10 @@
       <c r="E136" t="inlineStr"/>
       <c r="F136" t="inlineStr"/>
       <c r="G136" t="inlineStr"/>
-      <c r="H136" t="n">
-        <v>1.56474609375</v>
-      </c>
-      <c r="I136" t="inlineStr"/>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="n">
+        <v>0.57421875</v>
+      </c>
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr"/>
@@ -4441,10 +4377,10 @@
       <c r="E137" t="inlineStr"/>
       <c r="F137" t="inlineStr"/>
       <c r="G137" t="inlineStr"/>
-      <c r="H137" t="n">
-        <v>1.70830078125</v>
-      </c>
-      <c r="I137" t="inlineStr"/>
+      <c r="H137" t="inlineStr"/>
+      <c r="I137" t="n">
+        <v>0.64599609375</v>
+      </c>
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr"/>
@@ -4457,10 +4393,10 @@
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
-      <c r="H138" t="n">
-        <v>1.85185546875</v>
-      </c>
-      <c r="I138" t="inlineStr"/>
+      <c r="H138" t="inlineStr"/>
+      <c r="I138" t="n">
+        <v>0.70341796875</v>
+      </c>
       <c r="J138" t="inlineStr"/>
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr"/>
@@ -4473,10 +4409,10 @@
       <c r="E139" t="inlineStr"/>
       <c r="F139" t="inlineStr"/>
       <c r="G139" t="inlineStr"/>
-      <c r="H139" t="n">
-        <v>1.99541015625</v>
-      </c>
-      <c r="I139" t="inlineStr"/>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="n">
+        <v>0.861328125</v>
+      </c>
       <c r="J139" t="inlineStr"/>
       <c r="K139" t="inlineStr"/>
       <c r="L139" t="inlineStr"/>
@@ -4489,10 +4425,10 @@
       <c r="E140" t="inlineStr"/>
       <c r="F140" t="inlineStr"/>
       <c r="G140" t="inlineStr"/>
-      <c r="H140" t="n">
-        <v>2.11025390625</v>
-      </c>
-      <c r="I140" t="inlineStr"/>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="n">
+        <v>0.99052734375</v>
+      </c>
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr"/>
@@ -4505,10 +4441,10 @@
       <c r="E141" t="inlineStr"/>
       <c r="F141" t="inlineStr"/>
       <c r="G141" t="inlineStr"/>
-      <c r="H141" t="n">
-        <v>2.239453125</v>
-      </c>
-      <c r="I141" t="inlineStr"/>
+      <c r="H141" t="inlineStr"/>
+      <c r="I141" t="n">
+        <v>1.04794921875</v>
+      </c>
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr"/>
@@ -4521,10 +4457,10 @@
       <c r="E142" t="inlineStr"/>
       <c r="F142" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
-      <c r="H142" t="n">
-        <v>2.41171875</v>
-      </c>
-      <c r="I142" t="inlineStr"/>
+      <c r="H142" t="inlineStr"/>
+      <c r="I142" t="n">
+        <v>1.30634765625</v>
+      </c>
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr"/>
@@ -4537,10 +4473,10 @@
       <c r="E143" t="inlineStr"/>
       <c r="F143" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
-      <c r="H143" t="n">
-        <v>2.469140625</v>
-      </c>
-      <c r="I143" t="inlineStr"/>
+      <c r="H143" t="inlineStr"/>
+      <c r="I143" t="n">
+        <v>1.378125</v>
+      </c>
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr"/>
@@ -4553,10 +4489,10 @@
       <c r="E144" t="inlineStr"/>
       <c r="F144" t="inlineStr"/>
       <c r="G144" t="inlineStr"/>
-      <c r="H144" t="n">
-        <v>2.64140625</v>
-      </c>
-      <c r="I144" t="inlineStr"/>
+      <c r="H144" t="inlineStr"/>
+      <c r="I144" t="n">
+        <v>1.47861328125</v>
+      </c>
       <c r="J144" t="inlineStr"/>
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr"/>
@@ -4569,10 +4505,10 @@
       <c r="E145" t="inlineStr"/>
       <c r="F145" t="inlineStr"/>
       <c r="G145" t="inlineStr"/>
-      <c r="H145" t="n">
-        <v>2.9859375</v>
-      </c>
-      <c r="I145" t="inlineStr"/>
+      <c r="H145" t="inlineStr"/>
+      <c r="I145" t="n">
+        <v>1.550390625</v>
+      </c>
       <c r="J145" t="inlineStr"/>
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr"/>
@@ -4585,10 +4521,10 @@
       <c r="E146" t="inlineStr"/>
       <c r="F146" t="inlineStr"/>
       <c r="G146" t="inlineStr"/>
-      <c r="H146" t="n">
-        <v>3.54580078125</v>
-      </c>
-      <c r="I146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+      <c r="I146" t="n">
+        <v>1.62216796875</v>
+      </c>
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="inlineStr"/>
       <c r="L146" t="inlineStr"/>
@@ -4601,10 +4537,10 @@
       <c r="E147" t="inlineStr"/>
       <c r="F147" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
-      <c r="H147" t="n">
-        <v>4.34970703125</v>
-      </c>
-      <c r="I147" t="inlineStr"/>
+      <c r="H147" t="inlineStr"/>
+      <c r="I147" t="n">
+        <v>1.72265625</v>
+      </c>
       <c r="J147" t="inlineStr"/>
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr"/>
@@ -4617,10 +4553,10 @@
       <c r="E148" t="inlineStr"/>
       <c r="F148" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
-      <c r="H148" t="n">
-        <v>4.4501953125</v>
-      </c>
-      <c r="I148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
+      <c r="I148" t="n">
+        <v>1.79443359375</v>
+      </c>
       <c r="J148" t="inlineStr"/>
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr"/>
@@ -4633,10 +4569,10 @@
       <c r="E149" t="inlineStr"/>
       <c r="F149" t="inlineStr"/>
       <c r="G149" t="inlineStr"/>
-      <c r="H149" t="n">
-        <v>6.5748046875</v>
-      </c>
-      <c r="I149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
+      <c r="I149" t="n">
+        <v>1.894921875</v>
+      </c>
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr"/>
@@ -4651,7 +4587,7 @@
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="inlineStr"/>
       <c r="I150" t="n">
-        <v>0.30146484375</v>
+        <v>2.02412109375</v>
       </c>
       <c r="J150" t="inlineStr"/>
       <c r="K150" t="inlineStr"/>
@@ -4667,7 +4603,7 @@
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="inlineStr"/>
       <c r="I151" t="n">
-        <v>0.34453125</v>
+        <v>2.239453125</v>
       </c>
       <c r="J151" t="inlineStr"/>
       <c r="K151" t="inlineStr"/>
@@ -4683,7 +4619,7 @@
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="inlineStr"/>
       <c r="I152" t="n">
-        <v>0.57421875</v>
+        <v>2.75625</v>
       </c>
       <c r="J152" t="inlineStr"/>
       <c r="K152" t="inlineStr"/>
@@ -4699,7 +4635,7 @@
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="inlineStr"/>
       <c r="I153" t="n">
-        <v>0.64599609375</v>
+        <v>2.88544921875</v>
       </c>
       <c r="J153" t="inlineStr"/>
       <c r="K153" t="inlineStr"/>
@@ -4715,7 +4651,7 @@
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="inlineStr"/>
       <c r="I154" t="n">
-        <v>0.70341796875</v>
+        <v>3.043359375</v>
       </c>
       <c r="J154" t="inlineStr"/>
       <c r="K154" t="inlineStr"/>
@@ -4731,7 +4667,7 @@
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr"/>
       <c r="I155" t="n">
-        <v>0.861328125</v>
+        <v>3.17255859375</v>
       </c>
       <c r="J155" t="inlineStr"/>
       <c r="K155" t="inlineStr"/>
@@ -4747,7 +4683,7 @@
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="inlineStr"/>
       <c r="I156" t="n">
-        <v>0.90439453125</v>
+        <v>4.00517578125</v>
       </c>
       <c r="J156" t="inlineStr"/>
       <c r="K156" t="inlineStr"/>
@@ -4763,7 +4699,7 @@
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="inlineStr"/>
       <c r="I157" t="n">
-        <v>0.99052734375</v>
+        <v>4.17744140625</v>
       </c>
       <c r="J157" t="inlineStr"/>
       <c r="K157" t="inlineStr"/>
@@ -4778,10 +4714,10 @@
       <c r="F158" t="inlineStr"/>
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="inlineStr"/>
-      <c r="I158" t="n">
-        <v>1.04794921875</v>
-      </c>
-      <c r="J158" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" t="n">
+        <v>0.73212890625</v>
+      </c>
       <c r="K158" t="inlineStr"/>
       <c r="L158" t="inlineStr"/>
     </row>
@@ -4794,10 +4730,10 @@
       <c r="F159" t="inlineStr"/>
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="inlineStr"/>
-      <c r="I159" t="n">
-        <v>1.30634765625</v>
-      </c>
-      <c r="J159" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" t="n">
+        <v>0.78955078125</v>
+      </c>
       <c r="K159" t="inlineStr"/>
       <c r="L159" t="inlineStr"/>
     </row>
@@ -4810,10 +4746,10 @@
       <c r="F160" t="inlineStr"/>
       <c r="G160" t="inlineStr"/>
       <c r="H160" t="inlineStr"/>
-      <c r="I160" t="n">
-        <v>1.378125</v>
-      </c>
-      <c r="J160" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="n">
+        <v>0.84697265625</v>
+      </c>
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="inlineStr"/>
     </row>
@@ -4826,10 +4762,10 @@
       <c r="F161" t="inlineStr"/>
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="inlineStr"/>
-      <c r="I161" t="n">
-        <v>1.47861328125</v>
-      </c>
-      <c r="J161" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
+      <c r="J161" t="n">
+        <v>0.90439453125</v>
+      </c>
       <c r="K161" t="inlineStr"/>
       <c r="L161" t="inlineStr"/>
     </row>
@@ -4842,10 +4778,10 @@
       <c r="F162" t="inlineStr"/>
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="inlineStr"/>
-      <c r="I162" t="n">
-        <v>1.550390625</v>
-      </c>
-      <c r="J162" t="inlineStr"/>
+      <c r="I162" t="inlineStr"/>
+      <c r="J162" t="n">
+        <v>1.2345703125</v>
+      </c>
       <c r="K162" t="inlineStr"/>
       <c r="L162" t="inlineStr"/>
     </row>
@@ -4858,10 +4794,10 @@
       <c r="F163" t="inlineStr"/>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="inlineStr"/>
-      <c r="I163" t="n">
-        <v>1.62216796875</v>
-      </c>
-      <c r="J163" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
+      <c r="J163" t="n">
+        <v>1.435546875</v>
+      </c>
       <c r="K163" t="inlineStr"/>
       <c r="L163" t="inlineStr"/>
     </row>
@@ -4874,10 +4810,10 @@
       <c r="F164" t="inlineStr"/>
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="inlineStr"/>
-      <c r="I164" t="n">
-        <v>1.72265625</v>
-      </c>
-      <c r="J164" t="inlineStr"/>
+      <c r="I164" t="inlineStr"/>
+      <c r="J164" t="n">
+        <v>1.70830078125</v>
+      </c>
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr"/>
     </row>
@@ -4890,10 +4826,10 @@
       <c r="F165" t="inlineStr"/>
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="inlineStr"/>
-      <c r="I165" t="n">
-        <v>1.79443359375</v>
-      </c>
-      <c r="J165" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" t="n">
+        <v>1.96669921875</v>
+      </c>
       <c r="K165" t="inlineStr"/>
       <c r="L165" t="inlineStr"/>
     </row>
@@ -4906,10 +4842,10 @@
       <c r="F166" t="inlineStr"/>
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="inlineStr"/>
-      <c r="I166" t="n">
-        <v>1.894921875</v>
-      </c>
-      <c r="J166" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" t="n">
+        <v>3.56015625</v>
+      </c>
       <c r="K166" t="inlineStr"/>
       <c r="L166" t="inlineStr"/>
     </row>
@@ -4922,10 +4858,10 @@
       <c r="F167" t="inlineStr"/>
       <c r="G167" t="inlineStr"/>
       <c r="H167" t="inlineStr"/>
-      <c r="I167" t="n">
-        <v>2.02412109375</v>
-      </c>
-      <c r="J167" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+      <c r="J167" t="n">
+        <v>4.06259765625</v>
+      </c>
       <c r="K167" t="inlineStr"/>
       <c r="L167" t="inlineStr"/>
     </row>
@@ -4938,10 +4874,10 @@
       <c r="F168" t="inlineStr"/>
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="inlineStr"/>
-      <c r="I168" t="n">
-        <v>2.239453125</v>
-      </c>
-      <c r="J168" t="inlineStr"/>
+      <c r="I168" t="inlineStr"/>
+      <c r="J168" t="n">
+        <v>4.98134765625</v>
+      </c>
       <c r="K168" t="inlineStr"/>
       <c r="L168" t="inlineStr"/>
     </row>
@@ -4954,10 +4890,10 @@
       <c r="F169" t="inlineStr"/>
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="inlineStr"/>
-      <c r="I169" t="n">
-        <v>2.75625</v>
-      </c>
-      <c r="J169" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" t="n">
+        <v>7.27822265625</v>
+      </c>
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr"/>
     </row>
@@ -4970,11 +4906,11 @@
       <c r="F170" t="inlineStr"/>
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="inlineStr"/>
-      <c r="I170" t="n">
-        <v>2.88544921875</v>
-      </c>
+      <c r="I170" t="inlineStr"/>
       <c r="J170" t="inlineStr"/>
-      <c r="K170" t="inlineStr"/>
+      <c r="K170" t="n">
+        <v>0.287109375</v>
+      </c>
       <c r="L170" t="inlineStr"/>
     </row>
     <row r="171">
@@ -4986,11 +4922,11 @@
       <c r="F171" t="inlineStr"/>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="inlineStr"/>
-      <c r="I171" t="n">
-        <v>3.043359375</v>
-      </c>
+      <c r="I171" t="inlineStr"/>
       <c r="J171" t="inlineStr"/>
-      <c r="K171" t="inlineStr"/>
+      <c r="K171" t="n">
+        <v>0.73212890625</v>
+      </c>
       <c r="L171" t="inlineStr"/>
     </row>
     <row r="172">
@@ -5002,11 +4938,11 @@
       <c r="F172" t="inlineStr"/>
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="inlineStr"/>
-      <c r="I172" t="n">
-        <v>3.17255859375</v>
-      </c>
+      <c r="I172" t="inlineStr"/>
       <c r="J172" t="inlineStr"/>
-      <c r="K172" t="inlineStr"/>
+      <c r="K172" t="n">
+        <v>0.99052734375</v>
+      </c>
       <c r="L172" t="inlineStr"/>
     </row>
     <row r="173">
@@ -5018,11 +4954,11 @@
       <c r="F173" t="inlineStr"/>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="inlineStr"/>
-      <c r="I173" t="n">
-        <v>4.00517578125</v>
-      </c>
+      <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr"/>
-      <c r="K173" t="inlineStr"/>
+      <c r="K173" t="n">
+        <v>1.205859375</v>
+      </c>
       <c r="L173" t="inlineStr"/>
     </row>
     <row r="174">
@@ -5034,11 +4970,11 @@
       <c r="F174" t="inlineStr"/>
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="inlineStr"/>
-      <c r="I174" t="n">
-        <v>4.17744140625</v>
-      </c>
+      <c r="I174" t="inlineStr"/>
       <c r="J174" t="inlineStr"/>
-      <c r="K174" t="inlineStr"/>
+      <c r="K174" t="n">
+        <v>1.2919921875</v>
+      </c>
       <c r="L174" t="inlineStr"/>
     </row>
     <row r="175">
@@ -5051,10 +4987,10 @@
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="inlineStr"/>
       <c r="I175" t="inlineStr"/>
-      <c r="J175" t="n">
-        <v>0.6029296875</v>
-      </c>
-      <c r="K175" t="inlineStr"/>
+      <c r="J175" t="inlineStr"/>
+      <c r="K175" t="n">
+        <v>1.6365234375</v>
+      </c>
       <c r="L175" t="inlineStr"/>
     </row>
     <row r="176">
@@ -5067,10 +5003,10 @@
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="inlineStr"/>
       <c r="I176" t="inlineStr"/>
-      <c r="J176" t="n">
-        <v>0.73212890625</v>
-      </c>
-      <c r="K176" t="inlineStr"/>
+      <c r="J176" t="inlineStr"/>
+      <c r="K176" t="n">
+        <v>2.11025390625</v>
+      </c>
       <c r="L176" t="inlineStr"/>
     </row>
     <row r="177">
@@ -5083,10 +5019,10 @@
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="inlineStr"/>
       <c r="I177" t="inlineStr"/>
-      <c r="J177" t="n">
-        <v>0.78955078125</v>
-      </c>
-      <c r="K177" t="inlineStr"/>
+      <c r="J177" t="inlineStr"/>
+      <c r="K177" t="n">
+        <v>2.22509765625</v>
+      </c>
       <c r="L177" t="inlineStr"/>
     </row>
     <row r="178">
@@ -5099,10 +5035,10 @@
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="inlineStr"/>
       <c r="I178" t="inlineStr"/>
-      <c r="J178" t="n">
-        <v>0.84697265625</v>
-      </c>
-      <c r="K178" t="inlineStr"/>
+      <c r="J178" t="inlineStr"/>
+      <c r="K178" t="n">
+        <v>3.11513671875</v>
+      </c>
       <c r="L178" t="inlineStr"/>
     </row>
     <row r="179">
@@ -5115,10 +5051,10 @@
       <c r="G179" t="inlineStr"/>
       <c r="H179" t="inlineStr"/>
       <c r="I179" t="inlineStr"/>
-      <c r="J179" t="n">
-        <v>0.90439453125</v>
-      </c>
-      <c r="K179" t="inlineStr"/>
+      <c r="J179" t="inlineStr"/>
+      <c r="K179" t="n">
+        <v>5.01005859375</v>
+      </c>
       <c r="L179" t="inlineStr"/>
     </row>
     <row r="180">
@@ -5131,11 +5067,11 @@
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="inlineStr"/>
       <c r="I180" t="inlineStr"/>
-      <c r="J180" t="n">
-        <v>1.13408203125</v>
-      </c>
+      <c r="J180" t="inlineStr"/>
       <c r="K180" t="inlineStr"/>
-      <c r="L180" t="inlineStr"/>
+      <c r="L180" t="n">
+        <v>0.172265625</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr"/>
@@ -5147,11 +5083,11 @@
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="inlineStr"/>
       <c r="I181" t="inlineStr"/>
-      <c r="J181" t="n">
-        <v>1.2345703125</v>
-      </c>
+      <c r="J181" t="inlineStr"/>
       <c r="K181" t="inlineStr"/>
-      <c r="L181" t="inlineStr"/>
+      <c r="L181" t="n">
+        <v>0.34453125</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr"/>
@@ -5163,11 +5099,11 @@
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="inlineStr"/>
       <c r="I182" t="inlineStr"/>
-      <c r="J182" t="n">
-        <v>1.435546875</v>
-      </c>
+      <c r="J182" t="inlineStr"/>
       <c r="K182" t="inlineStr"/>
-      <c r="L182" t="inlineStr"/>
+      <c r="L182" t="n">
+        <v>0.516796875</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr"/>
@@ -5179,11 +5115,11 @@
       <c r="G183" t="inlineStr"/>
       <c r="H183" t="inlineStr"/>
       <c r="I183" t="inlineStr"/>
-      <c r="J183" t="n">
-        <v>1.70830078125</v>
-      </c>
+      <c r="J183" t="inlineStr"/>
       <c r="K183" t="inlineStr"/>
-      <c r="L183" t="inlineStr"/>
+      <c r="L183" t="n">
+        <v>1.2919921875</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr"/>
@@ -5195,11 +5131,11 @@
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="inlineStr"/>
       <c r="I184" t="inlineStr"/>
-      <c r="J184" t="n">
-        <v>1.96669921875</v>
-      </c>
+      <c r="J184" t="inlineStr"/>
       <c r="K184" t="inlineStr"/>
-      <c r="L184" t="inlineStr"/>
+      <c r="L184" t="n">
+        <v>1.5791015625</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr"/>
@@ -5211,11 +5147,11 @@
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="inlineStr"/>
       <c r="I185" t="inlineStr"/>
-      <c r="J185" t="n">
-        <v>3.56015625</v>
-      </c>
+      <c r="J185" t="inlineStr"/>
       <c r="K185" t="inlineStr"/>
-      <c r="L185" t="inlineStr"/>
+      <c r="L185" t="n">
+        <v>1.72265625</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr"/>
@@ -5227,11 +5163,11 @@
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="inlineStr"/>
       <c r="I186" t="inlineStr"/>
-      <c r="J186" t="n">
-        <v>4.06259765625</v>
-      </c>
+      <c r="J186" t="inlineStr"/>
       <c r="K186" t="inlineStr"/>
-      <c r="L186" t="inlineStr"/>
+      <c r="L186" t="n">
+        <v>1.8375</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr"/>
@@ -5243,11 +5179,11 @@
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="inlineStr"/>
       <c r="I187" t="inlineStr"/>
-      <c r="J187" t="n">
-        <v>4.20615234375</v>
-      </c>
+      <c r="J187" t="inlineStr"/>
       <c r="K187" t="inlineStr"/>
-      <c r="L187" t="inlineStr"/>
+      <c r="L187" t="n">
+        <v>2.33994140625</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr"/>
@@ -5259,11 +5195,11 @@
       <c r="G188" t="inlineStr"/>
       <c r="H188" t="inlineStr"/>
       <c r="I188" t="inlineStr"/>
-      <c r="J188" t="n">
-        <v>4.37841796875</v>
-      </c>
+      <c r="J188" t="inlineStr"/>
       <c r="K188" t="inlineStr"/>
-      <c r="L188" t="inlineStr"/>
+      <c r="L188" t="n">
+        <v>2.813671875</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr"/>
@@ -5275,11 +5211,11 @@
       <c r="G189" t="inlineStr"/>
       <c r="H189" t="inlineStr"/>
       <c r="I189" t="inlineStr"/>
-      <c r="J189" t="n">
-        <v>4.59375</v>
-      </c>
+      <c r="J189" t="inlineStr"/>
       <c r="K189" t="inlineStr"/>
-      <c r="L189" t="inlineStr"/>
+      <c r="L189" t="n">
+        <v>3.0720703125</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr"/>
@@ -5291,11 +5227,11 @@
       <c r="G190" t="inlineStr"/>
       <c r="H190" t="inlineStr"/>
       <c r="I190" t="inlineStr"/>
-      <c r="J190" t="n">
-        <v>4.98134765625</v>
-      </c>
+      <c r="J190" t="inlineStr"/>
       <c r="K190" t="inlineStr"/>
-      <c r="L190" t="inlineStr"/>
+      <c r="L190" t="n">
+        <v>3.40224609375</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr"/>
@@ -5307,11 +5243,11 @@
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="inlineStr"/>
       <c r="I191" t="inlineStr"/>
-      <c r="J191" t="n">
-        <v>7.27822265625</v>
-      </c>
+      <c r="J191" t="inlineStr"/>
       <c r="K191" t="inlineStr"/>
-      <c r="L191" t="inlineStr"/>
+      <c r="L191" t="n">
+        <v>4.0482421875</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr"/>
@@ -5324,10 +5260,10 @@
       <c r="H192" t="inlineStr"/>
       <c r="I192" t="inlineStr"/>
       <c r="J192" t="inlineStr"/>
-      <c r="K192" t="n">
-        <v>0.287109375</v>
-      </c>
-      <c r="L192" t="inlineStr"/>
+      <c r="K192" t="inlineStr"/>
+      <c r="L192" t="n">
+        <v>5.12490234375</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr"/>
@@ -5340,10 +5276,10 @@
       <c r="H193" t="inlineStr"/>
       <c r="I193" t="inlineStr"/>
       <c r="J193" t="inlineStr"/>
-      <c r="K193" t="n">
-        <v>0.73212890625</v>
-      </c>
-      <c r="L193" t="inlineStr"/>
+      <c r="K193" t="inlineStr"/>
+      <c r="L193" t="n">
+        <v>5.84267578125</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr"/>
@@ -5356,10 +5292,10 @@
       <c r="H194" t="inlineStr"/>
       <c r="I194" t="inlineStr"/>
       <c r="J194" t="inlineStr"/>
-      <c r="K194" t="n">
-        <v>0.99052734375</v>
-      </c>
-      <c r="L194" t="inlineStr"/>
+      <c r="K194" t="inlineStr"/>
+      <c r="L194" t="n">
+        <v>7.93857421875</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr"/>
@@ -5372,10 +5308,10 @@
       <c r="H195" t="inlineStr"/>
       <c r="I195" t="inlineStr"/>
       <c r="J195" t="inlineStr"/>
-      <c r="K195" t="n">
-        <v>1.205859375</v>
-      </c>
-      <c r="L195" t="inlineStr"/>
+      <c r="K195" t="inlineStr"/>
+      <c r="L195" t="n">
+        <v>8.311816406249999</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr"/>
@@ -5388,376 +5324,8 @@
       <c r="H196" t="inlineStr"/>
       <c r="I196" t="inlineStr"/>
       <c r="J196" t="inlineStr"/>
-      <c r="K196" t="n">
-        <v>1.2919921875</v>
-      </c>
-      <c r="L196" t="inlineStr"/>
-    </row>
-    <row r="197">
-      <c r="A197" t="inlineStr"/>
-      <c r="B197" t="inlineStr"/>
-      <c r="C197" t="inlineStr"/>
-      <c r="D197" t="inlineStr"/>
-      <c r="E197" t="inlineStr"/>
-      <c r="F197" t="inlineStr"/>
-      <c r="G197" t="inlineStr"/>
-      <c r="H197" t="inlineStr"/>
-      <c r="I197" t="inlineStr"/>
-      <c r="J197" t="inlineStr"/>
-      <c r="K197" t="n">
-        <v>1.6365234375</v>
-      </c>
-      <c r="L197" t="inlineStr"/>
-    </row>
-    <row r="198">
-      <c r="A198" t="inlineStr"/>
-      <c r="B198" t="inlineStr"/>
-      <c r="C198" t="inlineStr"/>
-      <c r="D198" t="inlineStr"/>
-      <c r="E198" t="inlineStr"/>
-      <c r="F198" t="inlineStr"/>
-      <c r="G198" t="inlineStr"/>
-      <c r="H198" t="inlineStr"/>
-      <c r="I198" t="inlineStr"/>
-      <c r="J198" t="inlineStr"/>
-      <c r="K198" t="n">
-        <v>2.11025390625</v>
-      </c>
-      <c r="L198" t="inlineStr"/>
-    </row>
-    <row r="199">
-      <c r="A199" t="inlineStr"/>
-      <c r="B199" t="inlineStr"/>
-      <c r="C199" t="inlineStr"/>
-      <c r="D199" t="inlineStr"/>
-      <c r="E199" t="inlineStr"/>
-      <c r="F199" t="inlineStr"/>
-      <c r="G199" t="inlineStr"/>
-      <c r="H199" t="inlineStr"/>
-      <c r="I199" t="inlineStr"/>
-      <c r="J199" t="inlineStr"/>
-      <c r="K199" t="n">
-        <v>2.22509765625</v>
-      </c>
-      <c r="L199" t="inlineStr"/>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr"/>
-      <c r="B200" t="inlineStr"/>
-      <c r="C200" t="inlineStr"/>
-      <c r="D200" t="inlineStr"/>
-      <c r="E200" t="inlineStr"/>
-      <c r="F200" t="inlineStr"/>
-      <c r="G200" t="inlineStr"/>
-      <c r="H200" t="inlineStr"/>
-      <c r="I200" t="inlineStr"/>
-      <c r="J200" t="inlineStr"/>
-      <c r="K200" t="n">
-        <v>3.11513671875</v>
-      </c>
-      <c r="L200" t="inlineStr"/>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr"/>
-      <c r="B201" t="inlineStr"/>
-      <c r="C201" t="inlineStr"/>
-      <c r="D201" t="inlineStr"/>
-      <c r="E201" t="inlineStr"/>
-      <c r="F201" t="inlineStr"/>
-      <c r="G201" t="inlineStr"/>
-      <c r="H201" t="inlineStr"/>
-      <c r="I201" t="inlineStr"/>
-      <c r="J201" t="inlineStr"/>
-      <c r="K201" t="n">
-        <v>5.01005859375</v>
-      </c>
-      <c r="L201" t="inlineStr"/>
-    </row>
-    <row r="202">
-      <c r="A202" t="inlineStr"/>
-      <c r="B202" t="inlineStr"/>
-      <c r="C202" t="inlineStr"/>
-      <c r="D202" t="inlineStr"/>
-      <c r="E202" t="inlineStr"/>
-      <c r="F202" t="inlineStr"/>
-      <c r="G202" t="inlineStr"/>
-      <c r="H202" t="inlineStr"/>
-      <c r="I202" t="inlineStr"/>
-      <c r="J202" t="inlineStr"/>
-      <c r="K202" t="inlineStr"/>
-      <c r="L202" t="n">
-        <v>0.172265625</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="inlineStr"/>
-      <c r="B203" t="inlineStr"/>
-      <c r="C203" t="inlineStr"/>
-      <c r="D203" t="inlineStr"/>
-      <c r="E203" t="inlineStr"/>
-      <c r="F203" t="inlineStr"/>
-      <c r="G203" t="inlineStr"/>
-      <c r="H203" t="inlineStr"/>
-      <c r="I203" t="inlineStr"/>
-      <c r="J203" t="inlineStr"/>
-      <c r="K203" t="inlineStr"/>
-      <c r="L203" t="n">
-        <v>0.34453125</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr"/>
-      <c r="B204" t="inlineStr"/>
-      <c r="C204" t="inlineStr"/>
-      <c r="D204" t="inlineStr"/>
-      <c r="E204" t="inlineStr"/>
-      <c r="F204" t="inlineStr"/>
-      <c r="G204" t="inlineStr"/>
-      <c r="H204" t="inlineStr"/>
-      <c r="I204" t="inlineStr"/>
-      <c r="J204" t="inlineStr"/>
-      <c r="K204" t="inlineStr"/>
-      <c r="L204" t="n">
-        <v>0.516796875</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="inlineStr"/>
-      <c r="B205" t="inlineStr"/>
-      <c r="C205" t="inlineStr"/>
-      <c r="D205" t="inlineStr"/>
-      <c r="E205" t="inlineStr"/>
-      <c r="F205" t="inlineStr"/>
-      <c r="G205" t="inlineStr"/>
-      <c r="H205" t="inlineStr"/>
-      <c r="I205" t="inlineStr"/>
-      <c r="J205" t="inlineStr"/>
-      <c r="K205" t="inlineStr"/>
-      <c r="L205" t="n">
-        <v>0.70341796875</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr"/>
-      <c r="B206" t="inlineStr"/>
-      <c r="C206" t="inlineStr"/>
-      <c r="D206" t="inlineStr"/>
-      <c r="E206" t="inlineStr"/>
-      <c r="F206" t="inlineStr"/>
-      <c r="G206" t="inlineStr"/>
-      <c r="H206" t="inlineStr"/>
-      <c r="I206" t="inlineStr"/>
-      <c r="J206" t="inlineStr"/>
-      <c r="K206" t="inlineStr"/>
-      <c r="L206" t="n">
-        <v>1.2919921875</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr"/>
-      <c r="B207" t="inlineStr"/>
-      <c r="C207" t="inlineStr"/>
-      <c r="D207" t="inlineStr"/>
-      <c r="E207" t="inlineStr"/>
-      <c r="F207" t="inlineStr"/>
-      <c r="G207" t="inlineStr"/>
-      <c r="H207" t="inlineStr"/>
-      <c r="I207" t="inlineStr"/>
-      <c r="J207" t="inlineStr"/>
-      <c r="K207" t="inlineStr"/>
-      <c r="L207" t="n">
-        <v>1.5791015625</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr"/>
-      <c r="B208" t="inlineStr"/>
-      <c r="C208" t="inlineStr"/>
-      <c r="D208" t="inlineStr"/>
-      <c r="E208" t="inlineStr"/>
-      <c r="F208" t="inlineStr"/>
-      <c r="G208" t="inlineStr"/>
-      <c r="H208" t="inlineStr"/>
-      <c r="I208" t="inlineStr"/>
-      <c r="J208" t="inlineStr"/>
-      <c r="K208" t="inlineStr"/>
-      <c r="L208" t="n">
-        <v>1.72265625</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr"/>
-      <c r="B209" t="inlineStr"/>
-      <c r="C209" t="inlineStr"/>
-      <c r="D209" t="inlineStr"/>
-      <c r="E209" t="inlineStr"/>
-      <c r="F209" t="inlineStr"/>
-      <c r="G209" t="inlineStr"/>
-      <c r="H209" t="inlineStr"/>
-      <c r="I209" t="inlineStr"/>
-      <c r="J209" t="inlineStr"/>
-      <c r="K209" t="inlineStr"/>
-      <c r="L209" t="n">
-        <v>1.8375</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr"/>
-      <c r="B210" t="inlineStr"/>
-      <c r="C210" t="inlineStr"/>
-      <c r="D210" t="inlineStr"/>
-      <c r="E210" t="inlineStr"/>
-      <c r="F210" t="inlineStr"/>
-      <c r="G210" t="inlineStr"/>
-      <c r="H210" t="inlineStr"/>
-      <c r="I210" t="inlineStr"/>
-      <c r="J210" t="inlineStr"/>
-      <c r="K210" t="inlineStr"/>
-      <c r="L210" t="n">
-        <v>2.33994140625</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr"/>
-      <c r="B211" t="inlineStr"/>
-      <c r="C211" t="inlineStr"/>
-      <c r="D211" t="inlineStr"/>
-      <c r="E211" t="inlineStr"/>
-      <c r="F211" t="inlineStr"/>
-      <c r="G211" t="inlineStr"/>
-      <c r="H211" t="inlineStr"/>
-      <c r="I211" t="inlineStr"/>
-      <c r="J211" t="inlineStr"/>
-      <c r="K211" t="inlineStr"/>
-      <c r="L211" t="n">
-        <v>2.813671875</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr"/>
-      <c r="B212" t="inlineStr"/>
-      <c r="C212" t="inlineStr"/>
-      <c r="D212" t="inlineStr"/>
-      <c r="E212" t="inlineStr"/>
-      <c r="F212" t="inlineStr"/>
-      <c r="G212" t="inlineStr"/>
-      <c r="H212" t="inlineStr"/>
-      <c r="I212" t="inlineStr"/>
-      <c r="J212" t="inlineStr"/>
-      <c r="K212" t="inlineStr"/>
-      <c r="L212" t="n">
-        <v>3.0720703125</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr"/>
-      <c r="B213" t="inlineStr"/>
-      <c r="C213" t="inlineStr"/>
-      <c r="D213" t="inlineStr"/>
-      <c r="E213" t="inlineStr"/>
-      <c r="F213" t="inlineStr"/>
-      <c r="G213" t="inlineStr"/>
-      <c r="H213" t="inlineStr"/>
-      <c r="I213" t="inlineStr"/>
-      <c r="J213" t="inlineStr"/>
-      <c r="K213" t="inlineStr"/>
-      <c r="L213" t="n">
-        <v>3.40224609375</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="inlineStr"/>
-      <c r="B214" t="inlineStr"/>
-      <c r="C214" t="inlineStr"/>
-      <c r="D214" t="inlineStr"/>
-      <c r="E214" t="inlineStr"/>
-      <c r="F214" t="inlineStr"/>
-      <c r="G214" t="inlineStr"/>
-      <c r="H214" t="inlineStr"/>
-      <c r="I214" t="inlineStr"/>
-      <c r="J214" t="inlineStr"/>
-      <c r="K214" t="inlineStr"/>
-      <c r="L214" t="n">
-        <v>4.0482421875</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="inlineStr"/>
-      <c r="B215" t="inlineStr"/>
-      <c r="C215" t="inlineStr"/>
-      <c r="D215" t="inlineStr"/>
-      <c r="E215" t="inlineStr"/>
-      <c r="F215" t="inlineStr"/>
-      <c r="G215" t="inlineStr"/>
-      <c r="H215" t="inlineStr"/>
-      <c r="I215" t="inlineStr"/>
-      <c r="J215" t="inlineStr"/>
-      <c r="K215" t="inlineStr"/>
-      <c r="L215" t="n">
-        <v>5.12490234375</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="inlineStr"/>
-      <c r="B216" t="inlineStr"/>
-      <c r="C216" t="inlineStr"/>
-      <c r="D216" t="inlineStr"/>
-      <c r="E216" t="inlineStr"/>
-      <c r="F216" t="inlineStr"/>
-      <c r="G216" t="inlineStr"/>
-      <c r="H216" t="inlineStr"/>
-      <c r="I216" t="inlineStr"/>
-      <c r="J216" t="inlineStr"/>
-      <c r="K216" t="inlineStr"/>
-      <c r="L216" t="n">
-        <v>5.84267578125</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="inlineStr"/>
-      <c r="B217" t="inlineStr"/>
-      <c r="C217" t="inlineStr"/>
-      <c r="D217" t="inlineStr"/>
-      <c r="E217" t="inlineStr"/>
-      <c r="F217" t="inlineStr"/>
-      <c r="G217" t="inlineStr"/>
-      <c r="H217" t="inlineStr"/>
-      <c r="I217" t="inlineStr"/>
-      <c r="J217" t="inlineStr"/>
-      <c r="K217" t="inlineStr"/>
-      <c r="L217" t="n">
-        <v>7.93857421875</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="inlineStr"/>
-      <c r="B218" t="inlineStr"/>
-      <c r="C218" t="inlineStr"/>
-      <c r="D218" t="inlineStr"/>
-      <c r="E218" t="inlineStr"/>
-      <c r="F218" t="inlineStr"/>
-      <c r="G218" t="inlineStr"/>
-      <c r="H218" t="inlineStr"/>
-      <c r="I218" t="inlineStr"/>
-      <c r="J218" t="inlineStr"/>
-      <c r="K218" t="inlineStr"/>
-      <c r="L218" t="n">
-        <v>8.311816406249999</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="inlineStr"/>
-      <c r="B219" t="inlineStr"/>
-      <c r="C219" t="inlineStr"/>
-      <c r="D219" t="inlineStr"/>
-      <c r="E219" t="inlineStr"/>
-      <c r="F219" t="inlineStr"/>
-      <c r="G219" t="inlineStr"/>
-      <c r="H219" t="inlineStr"/>
-      <c r="I219" t="inlineStr"/>
-      <c r="J219" t="inlineStr"/>
-      <c r="K219" t="inlineStr"/>
-      <c r="L219" t="n">
+      <c r="K196" t="inlineStr"/>
+      <c r="L196" t="n">
         <v>8.68505859375</v>
       </c>
     </row>

</xml_diff>